<commit_message>
Switch to using AB instead of PA
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fall 2015 09.16" sheetId="4" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>AB</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -546,39 +546,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
         <v>6</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
         <v>5</v>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -683,10 +683,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -718,46 +718,46 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:K6" si="0">SUM(B2:B5)</f>
-        <v>21</v>
+        <f t="shared" ref="B6" si="0">SUM(B2:B5)</f>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:K6" si="1">SUM(C2:C5)</f>
         <v>14</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -780,7 +780,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:T1048576"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -801,42 +801,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>2</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -903,10 +903,10 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5">
         <v>3</v>
@@ -973,46 +973,46 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:K6" si="0">SUM(B2:B5)</f>
-        <v>22</v>
+        <f t="shared" ref="B6" si="0">SUM(B2:B5)</f>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:K6" si="1">SUM(C2:C5)</f>
         <v>12</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:S1048576"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1056,42 +1056,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>4</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -1158,10 +1158,10 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
         <v>5</v>
@@ -1228,46 +1228,46 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:K6" si="0">SUM(B2:B5)</f>
-        <v>20</v>
+        <f t="shared" ref="B6" si="0">SUM(B2:B5)</f>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:K6" si="1">SUM(C2:C5)</f>
         <v>14</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1311,42 +1311,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>4</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5">
         <v>5</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
         <v>5</v>
@@ -1483,46 +1483,46 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:K6" si="0">SUM(B2:B5)</f>
-        <v>19</v>
+        <f t="shared" ref="B6" si="0">SUM(B2:B5)</f>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:K6" si="1">SUM(C2:C5)</f>
         <v>14</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1565,44 +1565,44 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3">
-        <f>4+3+4</f>
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <f>4+3+3</f>
+        <v>10</v>
       </c>
       <c r="C2" s="3">
         <f>1+1+2</f>
@@ -1639,11 +1639,11 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3">
-        <f>3+3+4</f>
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <f>3+2+3</f>
+        <v>8</v>
       </c>
       <c r="C3" s="3">
         <f>1+2+1</f>
@@ -1678,9 +1678,9 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
         <f t="shared" ref="B4" si="0">3+3+3</f>
         <v>9</v>
       </c>
@@ -1719,11 +1719,11 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3">
-        <f>4+3+4</f>
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
+        <f>4+3+3</f>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1760,9 +1760,9 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
         <f t="shared" ref="B6" si="4">3+3+4</f>
         <v>10</v>
       </c>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <f t="shared" ref="B7" si="5">3+3+3</f>
+        <v>15</v>
+      </c>
+      <c r="B7" s="5">
+        <f t="shared" ref="B7:B8" si="5">3+3+3</f>
         <v>9</v>
       </c>
       <c r="C7" s="3">
@@ -1836,10 +1836,10 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3">
-        <f t="shared" ref="B8" si="6">3+3+3</f>
+        <v>16</v>
+      </c>
+      <c r="B8" s="5">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="C8" s="3">
@@ -1874,14 +1874,14 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" ref="B9" si="7">4+3+3</f>
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <f t="shared" ref="B9" si="6">4+3+3</f>
         <v>10</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" ref="C9:C10" si="8">1+1</f>
+        <f t="shared" ref="C9:C10" si="7">1+1</f>
         <v>2</v>
       </c>
       <c r="D9" s="3">
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ref="F9:F10" si="9">1</f>
+        <f t="shared" ref="F9:F10" si="8">1</f>
         <v>1</v>
       </c>
       <c r="G9" s="3">
@@ -1913,14 +1913,14 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" ref="B10:B11" si="10">3+3+3</f>
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="5">
+        <f>3+1+3</f>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D10" s="3">
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G10" s="3">
@@ -1954,10 +1954,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="B11" s="5">
+        <f>3+3+3</f>
         <v>9</v>
       </c>
       <c r="C11" s="3">
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ref="H11:H12" si="11">1</f>
+        <f t="shared" ref="H11:H12" si="9">1</f>
         <v>1</v>
       </c>
       <c r="I11" s="3">
@@ -1994,10 +1994,10 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" ref="B12" si="12">1</f>
+        <v>21</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" ref="B12" si="10">1</f>
         <v>1</v>
       </c>
       <c r="C12" s="3">
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I12" s="3">
@@ -2032,46 +2032,46 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1">
-        <f t="shared" ref="B13:K13" si="13">SUM(B2:B12)</f>
-        <v>98</v>
+        <v>22</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" ref="B13" si="11">SUM(B2:B12)</f>
+        <v>92</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C13:K13" si="12">SUM(C2:C12)</f>
         <v>18</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>49</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
     </row>

</xml_diff>